<commit_message>
Controls / Camera work in most cases
- Strange behaviour on RESET
</commit_message>
<xml_diff>
--- a/08025-08975 Marks (compact) 17-18 (1).xlsx
+++ b/08025-08975 Marks (compact) 17-18 (1).xlsx
@@ -978,7 +978,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="D3" s="4">
         <f t="shared" ref="D3" si="0">SUMPRODUCT($C4:$C16,D4:D16)/SUM($C4:$C16)/10</f>
-        <v>0.578125</v>
+        <v>0.53125</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1076,7 +1076,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="38">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1100,7 +1100,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="38">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1148,7 +1148,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="38">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1160,7 +1160,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="38">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="D31" s="4">
         <f t="shared" ref="D31" si="1">SUMPRODUCT($C32:$C36,D32:D36)/SUM($C32:$C36)/10</f>
-        <v>0.7</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
@@ -1382,7 +1382,7 @@
         <v>1</v>
       </c>
       <c r="D35" s="38">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1393,7 +1393,7 @@
         <v>1</v>
       </c>
       <c r="D36" s="38">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1410,7 +1410,7 @@
       </c>
       <c r="D38" s="32">
         <f>(D3*$C3+D18*$C18)/($C3+$C18)</f>
-        <v>0.48359374999999993</v>
+        <v>0.44843749999999999</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="27" customFormat="1" x14ac:dyDescent="0.2">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="D39" s="29">
         <f t="shared" si="2"/>
-        <v>0.7</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -1436,7 +1436,7 @@
       </c>
       <c r="D40" s="20">
         <f>SUMPRODUCT($C38:$C39,D38:D39)</f>
-        <v>0.52687499999999998</v>
+        <v>0.52275000000000005</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1459,7 +1459,7 @@
       </c>
       <c r="D43" s="4">
         <f t="shared" ref="D43" si="3">D38</f>
-        <v>0.48359374999999993</v>
+        <v>0.44843749999999999</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1593,7 +1593,7 @@
       </c>
       <c r="D57" s="31">
         <f t="shared" ref="D57" si="6">D31</f>
-        <v>0.7</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.2">
@@ -1611,7 +1611,7 @@
       </c>
       <c r="D59" s="32">
         <f t="shared" ref="D59" si="7">D45*(D43*$C43 + (1-$C43 ))</f>
-        <v>0.63851562499999992</v>
+        <v>0.6139062500000001</v>
       </c>
     </row>
     <row r="60" spans="2:6" s="27" customFormat="1" x14ac:dyDescent="0.2">
@@ -1624,7 +1624,7 @@
       </c>
       <c r="D60" s="29">
         <f t="shared" ref="D60" si="8">D52*(D43*$C43 + (1-$C43 ))</f>
-        <v>0.63851562499999992</v>
+        <v>0.6139062500000001</v>
       </c>
     </row>
     <row r="61" spans="2:6" s="27" customFormat="1" x14ac:dyDescent="0.2">
@@ -1637,7 +1637,7 @@
       </c>
       <c r="D61" s="29">
         <f t="shared" si="9"/>
-        <v>0.7</v>
+        <v>0.82</v>
       </c>
     </row>
     <row r="62" spans="2:6" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -1650,7 +1650,7 @@
       </c>
       <c r="D62" s="20">
         <f t="shared" ref="D62" si="10">SUMPRODUCT($C59:$C61,D59:D61)</f>
-        <v>0.65081250000000002</v>
+        <v>0.65512500000000007</v>
       </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.2">

</xml_diff>